<commit_message>
Reverted and updated VCEA and 1.5 scenarios and policy schedules; updated trans/RTMF to reflect primarily reduction in VMT with only 5% of VMT change going to passenger rail.
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Virginia\Models\eps-virginia\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE4D269-1906-40C9-9438-66386A9FA2BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2250" windowWidth="23595" windowHeight="14160" xr2:uid="{B1321729-65FD-4E39-A16A-F420F6CD402A}"/>
+    <workbookView xWindow="3930" yWindow="2250" windowWidth="23595" windowHeight="14160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RTMF-passengers" sheetId="2" r:id="rId2"/>
     <sheet name="RTMF-freight" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -147,7 +146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -529,10 +528,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4A295D-ACEE-40E1-A0AB-57EEA1BFAA47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -659,7 +658,232 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5439016C-B89E-42B2-9367-3788A58F3CB4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="6">
+        <f t="shared" ref="I3:I7" si="0">1-SUM(B3:G3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -708,13 +932,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -725,7 +949,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="6">
         <f>1-SUM(B2:G2)</f>
-        <v>0.33999999999999997</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -742,10 +966,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -753,7 +977,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="6">
         <f t="shared" ref="I3:I7" si="0">1-SUM(B3:G3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -770,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -781,7 +1005,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="6">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -880,228 +1104,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E2AAAC-5DEA-4554-803B-E8EE05A805DF}">
-  <sheetPr>
-    <tabColor theme="4" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="6">
-        <f>1-SUM(B2:G2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="6">
-        <f t="shared" ref="I3:I7" si="0">1-SUM(B3:G3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>